<commit_message>
ukgov change again, bug fix and improvement
</commit_message>
<xml_diff>
--- a/nation.xlsx
+++ b/nation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\phe.gov.uk\porton\SharedData\ERD_Sci_Tech\GIS\PROJECTS AND INCIDENTS\Incidents\2020 Wuhan Coronavirus\AGOL\COVID19_Esri_AGOL_External\Processing\20200316\3_PRODUCTION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\phe.gov.uk\porton\SharedData\ERD_Sci_Tech\GIS\PROJECTS AND INCIDENTS\Incidents\2020 Wuhan Coronavirus\AGOL\COVID19_Esri_AGOL_External\Processing\20200318\3_PRODUCTION\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12036"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,6 +54,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="###,##0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,8 +115,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -433,15 +438,15 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="14.44140625" customWidth="1"/>
+    <col min="1" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,30 +472,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>43906</v>
+        <v>43908</v>
       </c>
       <c r="B2" s="4">
-        <v>1543</v>
+        <v>2626</v>
       </c>
       <c r="C2" s="4">
-        <v>152</v>
+        <v>676</v>
       </c>
       <c r="D2" s="4">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="E2" s="4">
-        <v>1196</v>
+        <v>2182</v>
       </c>
       <c r="F2" s="4">
-        <v>171</v>
+        <v>227</v>
       </c>
       <c r="G2" s="4">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="H2" s="4">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Northern Ireland changed its wording again, cool.
</commit_message>
<xml_diff>
--- a/nation.xlsx
+++ b/nation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\phe.gov.uk\porton\SharedData\ERD_Sci_Tech\GIS\PROJECTS AND INCIDENTS\Incidents\2020 Wuhan Coronavirus\AGOL\COVID19_Esri_AGOL_External\Processing\20200318\3_PRODUCTION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\phe.gov.uk\porton\SharedData\ERD_Sci_Tech\GIS\PROJECTS AND INCIDENTS\Incidents\2020 Wuhan Coronavirus\AGOL\COVID19_Esri_AGOL_External\Processing\20200319\3_PRODUCTION\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -119,6 +119,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -438,15 +441,15 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="8" width="14.42578125" customWidth="1"/>
+    <col min="1" max="8" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,30 +475,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
-        <v>43908</v>
+        <v>43909</v>
       </c>
       <c r="B2" s="4">
-        <v>2626</v>
+        <v>3269</v>
       </c>
       <c r="C2" s="4">
-        <v>676</v>
-      </c>
-      <c r="D2" s="4">
-        <v>103</v>
+        <v>643</v>
+      </c>
+      <c r="D2" s="5">
+        <v>144</v>
       </c>
       <c r="E2" s="4">
-        <v>2182</v>
+        <v>2756</v>
       </c>
       <c r="F2" s="4">
-        <v>227</v>
+        <v>266</v>
       </c>
       <c r="G2" s="4">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="H2" s="4">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
open second thread, hope it will work.
</commit_message>
<xml_diff>
--- a/nation.xlsx
+++ b/nation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\phe.gov.uk\porton\SharedData\ERD_Sci_Tech\GIS\PROJECTS AND INCIDENTS\Incidents\2020 Wuhan Coronavirus\AGOL\COVID19_Esri_AGOL_External\Processing\20200319\3_PRODUCTION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\phe.gov.uk\porton\SharedData\ERD_Sci_Tech\GIS\PROJECTS AND INCIDENTS\Incidents\2020 Wuhan Coronavirus\AGOL\COVID19_Esri_AGOL_External\Processing\20200321\3_PRODUCTION\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -54,9 +54,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="###,##0"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -115,15 +112,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,15 +430,15 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="14.453125" customWidth="1"/>
+    <col min="1" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,30 +464,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>43909</v>
-      </c>
-      <c r="B2" s="4">
-        <v>3269</v>
-      </c>
-      <c r="C2" s="4">
-        <v>643</v>
-      </c>
-      <c r="D2" s="5">
-        <v>144</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2756</v>
-      </c>
-      <c r="F2" s="4">
-        <v>266</v>
-      </c>
-      <c r="G2" s="4">
-        <v>170</v>
-      </c>
-      <c r="H2" s="4">
-        <v>77</v>
+        <v>43911</v>
+      </c>
+      <c r="B2">
+        <v>5018</v>
+      </c>
+      <c r="C2">
+        <v>1035</v>
+      </c>
+      <c r="D2">
+        <v>233</v>
+      </c>
+      <c r="E2">
+        <v>4257</v>
+      </c>
+      <c r="F2">
+        <v>373</v>
+      </c>
+      <c r="G2">
+        <v>280</v>
+      </c>
+      <c r="H2">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update readme, update death data source, update nIreland
</commit_message>
<xml_diff>
--- a/nation.xlsx
+++ b/nation.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12030"/>
   </bookViews>
@@ -48,23 +48,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="???,??0"/>
-    <numFmt numFmtId="170" formatCode="###,##0"/>
+    <numFmt numFmtId="164" formatCode="###,##0"/>
+    <numFmt numFmtId="165" formatCode="???,??0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -105,9 +100,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -117,19 +111,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -433,7 +426,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -444,12 +437,12 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="14.453125" customWidth="1"/>
+    <col min="1" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -478,30 +471,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
-        <v>43914</v>
-      </c>
-      <c r="B2" s="5">
-        <v>8077</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>43916</v>
+      </c>
+      <c r="B2" s="4">
+        <v>11658</v>
       </c>
       <c r="C2" s="5">
-        <v>1427</v>
-      </c>
-      <c r="D2" s="5">
-        <v>422</v>
-      </c>
-      <c r="E2" s="3">
-        <v>6843</v>
-      </c>
-      <c r="F2" s="5">
-        <v>584</v>
-      </c>
-      <c r="G2" s="5">
-        <v>478</v>
-      </c>
-      <c r="H2" s="5">
-        <v>172</v>
+        <v>2129</v>
+      </c>
+      <c r="D2" s="4">
+        <v>578</v>
+      </c>
+      <c r="E2" s="5">
+        <v>9782</v>
+      </c>
+      <c r="F2" s="4">
+        <v>894</v>
+      </c>
+      <c r="G2" s="4">
+        <v>741</v>
+      </c>
+      <c r="H2" s="4">
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update as uk gov publish tested number instead of negative
</commit_message>
<xml_diff>
--- a/nation.xlsx
+++ b/nation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12030"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>DateVal</t>
   </si>
@@ -43,12 +43,27 @@
   </si>
   <si>
     <t>NICases</t>
+  </si>
+  <si>
+    <t>DailyUKDeaths</t>
+  </si>
+  <si>
+    <t>EnglandDeaths</t>
+  </si>
+  <si>
+    <t>ScotlandDeaths</t>
+  </si>
+  <si>
+    <t>WalesDeaths</t>
+  </si>
+  <si>
+    <t>NIDeaths</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="###,##0"/>
     <numFmt numFmtId="165" formatCode="???,??0"/>
@@ -76,7 +91,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -94,6 +109,19 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -103,21 +131,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -426,7 +455,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -434,18 +463,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="14.42578125" customWidth="1"/>
+    <col min="1" max="8" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,47 +484,92 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>43916</v>
+        <v>43921</v>
       </c>
       <c r="B2" s="4">
-        <v>11658</v>
+        <v>25150</v>
       </c>
       <c r="C2" s="5">
-        <v>2129</v>
+        <v>3009</v>
       </c>
       <c r="D2" s="4">
-        <v>578</v>
-      </c>
-      <c r="E2" s="5">
-        <v>9782</v>
-      </c>
-      <c r="F2" s="4">
-        <v>894</v>
-      </c>
-      <c r="G2" s="4">
-        <v>741</v>
+        <v>1789</v>
+      </c>
+      <c r="E2" s="4">
+        <v>381</v>
+      </c>
+      <c r="F2" s="5">
+        <v>21008</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1651</v>
       </c>
       <c r="H2" s="4">
-        <v>241</v>
-      </c>
+        <v>1993</v>
+      </c>
+      <c r="I2" s="4">
+        <v>47</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1563</v>
+      </c>
+      <c r="K2" s="4">
+        <v>69</v>
+      </c>
+      <c r="L2" s="4">
+        <v>586</v>
+      </c>
+      <c r="M2" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
improve wales, update readme
</commit_message>
<xml_diff>
--- a/nation.xlsx
+++ b/nation.xlsx
@@ -77,18 +77,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -131,22 +125,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -469,12 +460,12 @@
       <selection activeCell="A2" sqref="A2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="14.44140625" customWidth="1"/>
+    <col min="1" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,48 +506,48 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>43921</v>
+        <v>43923</v>
       </c>
       <c r="B2" s="4">
-        <v>25150</v>
+        <v>33718</v>
       </c>
       <c r="C2" s="5">
-        <v>3009</v>
+        <v>4244</v>
       </c>
       <c r="D2" s="4">
-        <v>1789</v>
+        <v>2921</v>
       </c>
       <c r="E2" s="4">
-        <v>381</v>
+        <v>569</v>
       </c>
       <c r="F2" s="5">
-        <v>21008</v>
-      </c>
-      <c r="G2" s="6">
-        <v>1651</v>
+        <v>28221</v>
+      </c>
+      <c r="G2" s="5">
+        <v>2698</v>
       </c>
       <c r="H2" s="4">
-        <v>1993</v>
+        <v>2602</v>
       </c>
       <c r="I2" s="4">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="J2" s="4">
-        <v>1563</v>
+        <v>2121</v>
       </c>
       <c r="K2" s="4">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="L2" s="4">
-        <v>586</v>
+        <v>774</v>
       </c>
       <c r="M2" s="4">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>

</xml_diff>

<commit_message>
Due to the statistical changes, test data increse and positive rate appears not lining up with the government's figure, some fix and save number of tested done
</commit_message>
<xml_diff>
--- a/nation.xlsx
+++ b/nation.xlsx
@@ -65,10 +65,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="###,##0"/>
-    <numFmt numFmtId="165" formatCode="???,??0"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="##,##0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,10 +129,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -134,14 +142,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -456,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,43 +514,43 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>43923</v>
+        <v>43928</v>
       </c>
       <c r="B2" s="4">
-        <v>33718</v>
-      </c>
-      <c r="C2" s="5">
-        <v>4244</v>
+        <v>55242</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3634</v>
       </c>
       <c r="D2" s="4">
-        <v>2921</v>
+        <v>6159</v>
       </c>
       <c r="E2" s="4">
-        <v>569</v>
-      </c>
-      <c r="F2" s="5">
-        <v>28221</v>
-      </c>
-      <c r="G2" s="5">
-        <v>2698</v>
+        <v>786</v>
+      </c>
+      <c r="F2" s="4">
+        <v>42990</v>
+      </c>
+      <c r="G2" s="4">
+        <v>4897</v>
       </c>
       <c r="H2" s="4">
-        <v>2602</v>
+        <v>3961</v>
       </c>
       <c r="I2" s="4">
-        <v>76</v>
+        <v>220</v>
       </c>
       <c r="J2" s="4">
-        <v>2121</v>
+        <v>3499</v>
       </c>
       <c r="K2" s="4">
-        <v>117</v>
+        <v>193</v>
       </c>
       <c r="L2" s="4">
-        <v>774</v>
+        <v>1158</v>
       </c>
       <c r="M2" s="4">
-        <v>30</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix scotland, add gov update  timeline
</commit_message>
<xml_diff>
--- a/nation.xlsx
+++ b/nation.xlsx
@@ -66,7 +66,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="##,##0"/>
+    <numFmt numFmtId="166" formatCode="##,##0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -142,7 +142,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -463,15 +463,15 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="8" width="14.42578125" customWidth="1"/>
+    <col min="1" max="8" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,48 +512,48 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
-        <v>43928</v>
+        <v>43929</v>
       </c>
       <c r="B2" s="4">
-        <v>55242</v>
+        <v>60733</v>
       </c>
       <c r="C2" s="4">
-        <v>3634</v>
+        <v>5491</v>
       </c>
       <c r="D2" s="4">
-        <v>6159</v>
+        <v>7097</v>
       </c>
       <c r="E2" s="4">
-        <v>786</v>
+        <v>938</v>
       </c>
       <c r="F2" s="4">
-        <v>42990</v>
+        <v>50756</v>
       </c>
       <c r="G2" s="4">
-        <v>4897</v>
+        <v>6483</v>
       </c>
       <c r="H2" s="4">
-        <v>3961</v>
+        <v>4565</v>
       </c>
       <c r="I2" s="4">
-        <v>220</v>
+        <v>296</v>
       </c>
       <c r="J2" s="4">
-        <v>3499</v>
+        <v>4073</v>
       </c>
       <c r="K2" s="4">
-        <v>193</v>
+        <v>245</v>
       </c>
       <c r="L2" s="4">
-        <v>1158</v>
+        <v>1339</v>
       </c>
       <c r="M2" s="4">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>

</xml_diff>

<commit_message>
deal with , in number
</commit_message>
<xml_diff>
--- a/nation.xlsx
+++ b/nation.xlsx
@@ -64,11 +64,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="##,##0"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="###,##0"/>
+    <numFmt numFmtId="165" formatCode="???,??0"/>
+    <numFmt numFmtId="166" formatCode="?,??0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,18 +79,35 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -131,23 +149,32 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -463,7 +490,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,43 +541,43 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
-        <v>43929</v>
+        <v>43931</v>
       </c>
       <c r="B2" s="4">
-        <v>60733</v>
-      </c>
-      <c r="C2" s="4">
-        <v>5491</v>
-      </c>
-      <c r="D2" s="4">
-        <v>7097</v>
-      </c>
-      <c r="E2" s="4">
-        <v>938</v>
-      </c>
-      <c r="F2" s="4">
-        <v>50756</v>
-      </c>
-      <c r="G2" s="4">
-        <v>6483</v>
-      </c>
-      <c r="H2" s="4">
-        <v>4565</v>
-      </c>
-      <c r="I2" s="4">
-        <v>296</v>
-      </c>
-      <c r="J2" s="4">
-        <v>4073</v>
-      </c>
-      <c r="K2" s="4">
-        <v>245</v>
-      </c>
-      <c r="L2" s="4">
-        <v>1339</v>
-      </c>
-      <c r="M2" s="4">
-        <v>73</v>
+        <v>70272</v>
+      </c>
+      <c r="C2" s="5">
+        <v>5195</v>
+      </c>
+      <c r="D2" s="6">
+        <v>8958</v>
+      </c>
+      <c r="E2" s="6">
+        <v>980</v>
+      </c>
+      <c r="F2" s="7">
+        <v>58817</v>
+      </c>
+      <c r="G2" s="5">
+        <v>8114</v>
+      </c>
+      <c r="H2" s="6">
+        <v>5275</v>
+      </c>
+      <c r="I2" s="6">
+        <v>447</v>
+      </c>
+      <c r="J2" s="6">
+        <v>4591</v>
+      </c>
+      <c r="K2" s="6">
+        <v>315</v>
+      </c>
+      <c r="L2" s="6">
+        <v>1589</v>
+      </c>
+      <c r="M2" s="6">
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
remove front and back space for scot area location name
</commit_message>
<xml_diff>
--- a/nation.xlsx
+++ b/nation.xlsx
@@ -105,7 +105,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,13 +151,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -166,10 +166,13 @@
     <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -490,15 +493,15 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="14.453125" customWidth="1"/>
+    <col min="1" max="8" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,48 +542,48 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>43931</v>
+        <v>43932</v>
       </c>
       <c r="B2" s="4">
-        <v>70272</v>
+        <v>78991</v>
       </c>
       <c r="C2" s="5">
-        <v>5195</v>
+        <v>5234</v>
       </c>
       <c r="D2" s="6">
-        <v>8958</v>
+        <v>9875</v>
       </c>
       <c r="E2" s="6">
-        <v>980</v>
+        <v>917</v>
       </c>
       <c r="F2" s="7">
-        <v>58817</v>
-      </c>
-      <c r="G2" s="5">
-        <v>8114</v>
+        <v>62658</v>
+      </c>
+      <c r="G2" s="8">
+        <v>8937</v>
       </c>
       <c r="H2" s="6">
-        <v>5275</v>
+        <v>5590</v>
       </c>
       <c r="I2" s="6">
-        <v>447</v>
+        <v>495</v>
       </c>
       <c r="J2" s="6">
-        <v>4591</v>
+        <v>4930</v>
       </c>
       <c r="K2" s="6">
-        <v>315</v>
+        <v>351</v>
       </c>
       <c r="L2" s="6">
-        <v>1589</v>
+        <v>1717</v>
       </c>
       <c r="M2" s="6">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>

</xml_diff>